<commit_message>
endret dataset og litt i ontologien
</commit_message>
<xml_diff>
--- a/Datasett/Nye datasett/Kirker.xlsx
+++ b/Datasett/Nye datasett/Kirker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marte\Documents\uib\6. semester\INFO216 Advanced Modelling\Project_Y\Datasett\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marte\Documents\uib\6. semester\INFO216 Advanced Modelling\Project_Y\Datasett\Nye datasett\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1003,7 +1003,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1173,7 +1173,7 @@
         <v>45</v>
       </c>
       <c r="G6">
-        <v>2270</v>
+        <v>490</v>
       </c>
       <c r="H6">
         <v>4335</v>

</xml_diff>